<commit_message>
Login contra Tabla del Server
</commit_message>
<xml_diff>
--- a/Documentos/Omexon desvaríos iniciales.xlsx
+++ b/Documentos/Omexon desvaríos iniciales.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Xamarin\OmexomApp\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{40C45280-3F62-491A-8E73-95F9485BDDDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B200FD-8076-44A0-B878-7DB76C7E40CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E1B8A5DC-F207-4BE4-8157-6442224232A7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E1B8A5DC-F207-4BE4-8157-6442224232A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="78">
   <si>
     <t>OT</t>
   </si>
@@ -287,6 +288,21 @@
   </si>
   <si>
     <t>Fechasinconizacion</t>
+  </si>
+  <si>
+    <t>Tabla</t>
+  </si>
+  <si>
+    <t>SubContratistasUsrWeb</t>
+  </si>
+  <si>
+    <t>Si hay Internet, bajar a tabla Local esta tabla</t>
+  </si>
+  <si>
+    <t>Si la Tabla Local tiene filas, chequear Usuario y Password contra esta tabla</t>
+  </si>
+  <si>
+    <t>Ingresar a HomePage</t>
   </si>
 </sst>
 </file>
@@ -783,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B18FCCD-6FB3-424A-BEF2-93531F064B77}">
   <dimension ref="B1:R83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E81" sqref="E81"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1495,4 +1511,42 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63010D2E-2B55-4B03-ABA5-D4E20B049743}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>